<commit_message>
Cleared data for document attachments as of now boz of execution time but logic is implemented.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForReview-CancelAndClose.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForReview-CancelAndClose.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>To</t>
   </si>
@@ -88,15 +88,6 @@
   </si>
   <si>
     <t>Close</t>
-  </si>
-  <si>
-    <t>Document Register</t>
-  </si>
-  <si>
-    <t>Test 1 ta.docx</t>
-  </si>
-  <si>
-    <t>BrowseDocument.docx</t>
   </si>
   <si>
     <t>Cancel</t>
@@ -511,9 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -586,10 +575,10 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -605,21 +594,6 @@
       </c>
       <c r="G2" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
       </c>
       <c r="M2" t="s">
         <v>5</v>
@@ -630,10 +604,10 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -650,31 +624,16 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
       <c r="M3" t="s">
         <v>5</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -690,21 +649,6 @@
       </c>
       <c r="G4" t="s">
         <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
       </c>
       <c r="M4" t="s">
         <v>5</v>
@@ -715,7 +659,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -732,26 +676,11 @@
       <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" t="s">
-        <v>25</v>
-      </c>
       <c r="M5" t="s">
         <v>5</v>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>